<commit_message>
Added Keck logo as background and bootstrap styling - not complete yet
</commit_message>
<xml_diff>
--- a/dropdowns.xlsx
+++ b/dropdowns.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\FlaskApp\Login\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\FlaskApp\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA2A2AA-7F76-4D7A-8E25-5B393A82EE63}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DC8704-0EE0-4C23-8F1E-6BC5F07A7899}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{F953016D-5165-4C1A-B7E7-E58E4312BF90}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Pedigree</t>
   </si>
@@ -75,10 +75,13 @@
     <t>Compression</t>
   </si>
   <si>
-    <t>Carlos</t>
-  </si>
-  <si>
     <t>Issac</t>
+  </si>
+  <si>
+    <t>Filament: ABS</t>
+  </si>
+  <si>
+    <t>Filament: Ultem</t>
   </si>
 </sst>
 </file>
@@ -439,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D24C04-8227-4AF6-95CA-05577D7AFF3E}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,15 +509,20 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Elastic search working and displaying results on search page, need to format results
</commit_message>
<xml_diff>
--- a/dropdowns.xlsx
+++ b/dropdowns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\FlaskApp\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DC8704-0EE0-4C23-8F1E-6BC5F07A7899}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C38AA82-01FA-43E8-8152-0F4A10BD6036}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{F953016D-5165-4C1A-B7E7-E58E4312BF90}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Pedigree</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Filament: Ultem</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
   </si>
 </sst>
 </file>
@@ -442,18 +445,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D24C04-8227-4AF6-95CA-05577D7AFF3E}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -472,56 +475,70 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>